<commit_message>
feat: Add thermal data for 244,5х6,3 column size in both XLSX and JSON formats.
</commit_message>
<xml_diff>
--- a/thermal xlm/244,5х6,3.xlsx
+++ b/thermal xlm/244,5х6,3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\01_Postgraduate\Статьи\ВАК\ВАК Пожары и ЧС3 Сталебетон\Python program_V2\fire_column_app\thermal xlm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B716A-CF36-46F8-8A35-30F311CAD7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0869FA66-7CF5-4037-ADBF-FF84D5FE1F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EEF9BC8-23BF-450E-9042-F798D29F0F82}"/>
   </bookViews>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EB8B82-DEFF-4CFC-9AAE-C98B3F9C19FD}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q92" sqref="Q92"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,6 +3368,4806 @@
         <v>306.87</v>
       </c>
     </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>5460</v>
+      </c>
+      <c r="B93">
+        <v>947.94</v>
+      </c>
+      <c r="C93">
+        <v>876.35</v>
+      </c>
+      <c r="D93">
+        <v>694.07</v>
+      </c>
+      <c r="E93">
+        <v>532.59</v>
+      </c>
+      <c r="F93">
+        <v>532.6</v>
+      </c>
+      <c r="G93">
+        <v>430.24</v>
+      </c>
+      <c r="H93">
+        <v>357.86</v>
+      </c>
+      <c r="I93">
+        <v>320.32</v>
+      </c>
+      <c r="J93">
+        <v>311.64999999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>5520</v>
+      </c>
+      <c r="B94">
+        <v>950.13</v>
+      </c>
+      <c r="C94">
+        <v>879.09</v>
+      </c>
+      <c r="D94">
+        <v>697.84</v>
+      </c>
+      <c r="E94">
+        <v>536.87</v>
+      </c>
+      <c r="F94">
+        <v>536.88</v>
+      </c>
+      <c r="G94">
+        <v>434.75</v>
+      </c>
+      <c r="H94">
+        <v>362.48</v>
+      </c>
+      <c r="I94">
+        <v>325.02999999999997</v>
+      </c>
+      <c r="J94">
+        <v>316.38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>5580</v>
+      </c>
+      <c r="B95">
+        <v>952.29</v>
+      </c>
+      <c r="C95">
+        <v>881.8</v>
+      </c>
+      <c r="D95">
+        <v>701.57</v>
+      </c>
+      <c r="E95">
+        <v>541.12</v>
+      </c>
+      <c r="F95">
+        <v>541.13</v>
+      </c>
+      <c r="G95">
+        <v>439.23</v>
+      </c>
+      <c r="H95">
+        <v>367.07</v>
+      </c>
+      <c r="I95">
+        <v>329.69</v>
+      </c>
+      <c r="J95">
+        <v>321.06</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>5640</v>
+      </c>
+      <c r="B96">
+        <v>954.43</v>
+      </c>
+      <c r="C96">
+        <v>884.48</v>
+      </c>
+      <c r="D96">
+        <v>705.26</v>
+      </c>
+      <c r="E96">
+        <v>545.33000000000004</v>
+      </c>
+      <c r="F96">
+        <v>545.34</v>
+      </c>
+      <c r="G96">
+        <v>443.67</v>
+      </c>
+      <c r="H96">
+        <v>371.62</v>
+      </c>
+      <c r="I96">
+        <v>334.31</v>
+      </c>
+      <c r="J96">
+        <v>325.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>5700</v>
+      </c>
+      <c r="B97">
+        <v>956.53</v>
+      </c>
+      <c r="C97">
+        <v>887.12</v>
+      </c>
+      <c r="D97">
+        <v>708.91</v>
+      </c>
+      <c r="E97">
+        <v>549.5</v>
+      </c>
+      <c r="F97">
+        <v>549.51</v>
+      </c>
+      <c r="G97">
+        <v>448.07</v>
+      </c>
+      <c r="H97">
+        <v>376.13</v>
+      </c>
+      <c r="I97">
+        <v>338.88</v>
+      </c>
+      <c r="J97">
+        <v>330.29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>5760</v>
+      </c>
+      <c r="B98">
+        <v>958.61</v>
+      </c>
+      <c r="C98">
+        <v>889.73</v>
+      </c>
+      <c r="D98">
+        <v>712.53</v>
+      </c>
+      <c r="E98">
+        <v>553.64</v>
+      </c>
+      <c r="F98">
+        <v>553.65</v>
+      </c>
+      <c r="G98">
+        <v>452.45</v>
+      </c>
+      <c r="H98">
+        <v>380.6</v>
+      </c>
+      <c r="I98">
+        <v>343.42</v>
+      </c>
+      <c r="J98">
+        <v>334.84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>5820</v>
+      </c>
+      <c r="B99">
+        <v>960.65</v>
+      </c>
+      <c r="C99">
+        <v>892.3</v>
+      </c>
+      <c r="D99">
+        <v>716.11</v>
+      </c>
+      <c r="E99">
+        <v>557.75</v>
+      </c>
+      <c r="F99">
+        <v>557.76</v>
+      </c>
+      <c r="G99">
+        <v>456.79</v>
+      </c>
+      <c r="H99">
+        <v>385.04</v>
+      </c>
+      <c r="I99">
+        <v>347.91</v>
+      </c>
+      <c r="J99">
+        <v>339.35</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>5880</v>
+      </c>
+      <c r="B100">
+        <v>962.67</v>
+      </c>
+      <c r="C100">
+        <v>894.85</v>
+      </c>
+      <c r="D100">
+        <v>719.65</v>
+      </c>
+      <c r="E100">
+        <v>561.82000000000005</v>
+      </c>
+      <c r="F100">
+        <v>561.83000000000004</v>
+      </c>
+      <c r="G100">
+        <v>461.09</v>
+      </c>
+      <c r="H100">
+        <v>389.44</v>
+      </c>
+      <c r="I100">
+        <v>352.36</v>
+      </c>
+      <c r="J100">
+        <v>343.82</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>5940</v>
+      </c>
+      <c r="B101">
+        <v>964.67</v>
+      </c>
+      <c r="C101">
+        <v>897.36</v>
+      </c>
+      <c r="D101">
+        <v>723.16</v>
+      </c>
+      <c r="E101">
+        <v>565.85</v>
+      </c>
+      <c r="F101">
+        <v>565.86</v>
+      </c>
+      <c r="G101">
+        <v>465.36</v>
+      </c>
+      <c r="H101">
+        <v>393.82</v>
+      </c>
+      <c r="I101">
+        <v>356.77</v>
+      </c>
+      <c r="J101">
+        <v>348.25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>6000</v>
+      </c>
+      <c r="B102">
+        <v>966.64</v>
+      </c>
+      <c r="C102">
+        <v>899.85</v>
+      </c>
+      <c r="D102">
+        <v>726.63</v>
+      </c>
+      <c r="E102">
+        <v>569.86</v>
+      </c>
+      <c r="F102">
+        <v>569.87</v>
+      </c>
+      <c r="G102">
+        <v>469.6</v>
+      </c>
+      <c r="H102">
+        <v>398.16</v>
+      </c>
+      <c r="I102">
+        <v>361.15</v>
+      </c>
+      <c r="J102">
+        <v>352.64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>6060</v>
+      </c>
+      <c r="B103">
+        <v>968.58</v>
+      </c>
+      <c r="C103">
+        <v>902.3</v>
+      </c>
+      <c r="D103">
+        <v>730.06</v>
+      </c>
+      <c r="E103">
+        <v>573.83000000000004</v>
+      </c>
+      <c r="F103">
+        <v>573.84</v>
+      </c>
+      <c r="G103">
+        <v>473.81</v>
+      </c>
+      <c r="H103">
+        <v>402.47</v>
+      </c>
+      <c r="I103">
+        <v>365.49</v>
+      </c>
+      <c r="J103">
+        <v>356.99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>6120</v>
+      </c>
+      <c r="B104">
+        <v>970.5</v>
+      </c>
+      <c r="C104">
+        <v>904.72</v>
+      </c>
+      <c r="D104">
+        <v>733.46</v>
+      </c>
+      <c r="E104">
+        <v>577.77</v>
+      </c>
+      <c r="F104">
+        <v>577.78</v>
+      </c>
+      <c r="G104">
+        <v>477.99</v>
+      </c>
+      <c r="H104">
+        <v>406.75</v>
+      </c>
+      <c r="I104">
+        <v>369.79</v>
+      </c>
+      <c r="J104">
+        <v>361.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>6180</v>
+      </c>
+      <c r="B105">
+        <v>972.4</v>
+      </c>
+      <c r="C105">
+        <v>907.12</v>
+      </c>
+      <c r="D105">
+        <v>736.83</v>
+      </c>
+      <c r="E105">
+        <v>581.66999999999996</v>
+      </c>
+      <c r="F105">
+        <v>581.67999999999995</v>
+      </c>
+      <c r="G105">
+        <v>482.14</v>
+      </c>
+      <c r="H105">
+        <v>411</v>
+      </c>
+      <c r="I105">
+        <v>374.07</v>
+      </c>
+      <c r="J105">
+        <v>365.58</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>6240</v>
+      </c>
+      <c r="B106">
+        <v>974.27</v>
+      </c>
+      <c r="C106">
+        <v>909.48</v>
+      </c>
+      <c r="D106">
+        <v>740.16</v>
+      </c>
+      <c r="E106">
+        <v>585.54999999999995</v>
+      </c>
+      <c r="F106">
+        <v>585.55999999999995</v>
+      </c>
+      <c r="G106">
+        <v>486.26</v>
+      </c>
+      <c r="H106">
+        <v>415.22</v>
+      </c>
+      <c r="I106">
+        <v>378.3</v>
+      </c>
+      <c r="J106">
+        <v>369.83</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>6300</v>
+      </c>
+      <c r="B107">
+        <v>976.12</v>
+      </c>
+      <c r="C107">
+        <v>911.82</v>
+      </c>
+      <c r="D107">
+        <v>743.46</v>
+      </c>
+      <c r="E107">
+        <v>589.39</v>
+      </c>
+      <c r="F107">
+        <v>589.41</v>
+      </c>
+      <c r="G107">
+        <v>490.34</v>
+      </c>
+      <c r="H107">
+        <v>419.41</v>
+      </c>
+      <c r="I107">
+        <v>382.51</v>
+      </c>
+      <c r="J107">
+        <v>374.04</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>6360</v>
+      </c>
+      <c r="B108">
+        <v>977.95</v>
+      </c>
+      <c r="C108">
+        <v>914.13</v>
+      </c>
+      <c r="D108">
+        <v>746.73</v>
+      </c>
+      <c r="E108">
+        <v>593.21</v>
+      </c>
+      <c r="F108">
+        <v>593.22</v>
+      </c>
+      <c r="G108">
+        <v>494.4</v>
+      </c>
+      <c r="H108">
+        <v>423.57</v>
+      </c>
+      <c r="I108">
+        <v>386.69</v>
+      </c>
+      <c r="J108">
+        <v>378.22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>6420</v>
+      </c>
+      <c r="B109">
+        <v>979.76</v>
+      </c>
+      <c r="C109">
+        <v>916.41</v>
+      </c>
+      <c r="D109">
+        <v>749.96</v>
+      </c>
+      <c r="E109">
+        <v>597</v>
+      </c>
+      <c r="F109">
+        <v>597.01</v>
+      </c>
+      <c r="G109">
+        <v>498.43</v>
+      </c>
+      <c r="H109">
+        <v>427.71</v>
+      </c>
+      <c r="I109">
+        <v>390.83</v>
+      </c>
+      <c r="J109">
+        <v>382.37</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>6480</v>
+      </c>
+      <c r="B110">
+        <v>981.54</v>
+      </c>
+      <c r="C110">
+        <v>918.67</v>
+      </c>
+      <c r="D110">
+        <v>753.17</v>
+      </c>
+      <c r="E110">
+        <v>600.75</v>
+      </c>
+      <c r="F110">
+        <v>600.76</v>
+      </c>
+      <c r="G110">
+        <v>502.44</v>
+      </c>
+      <c r="H110">
+        <v>431.81</v>
+      </c>
+      <c r="I110">
+        <v>394.95</v>
+      </c>
+      <c r="J110">
+        <v>386.49</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>6540</v>
+      </c>
+      <c r="B111">
+        <v>983.31</v>
+      </c>
+      <c r="C111">
+        <v>920.9</v>
+      </c>
+      <c r="D111">
+        <v>756.34</v>
+      </c>
+      <c r="E111">
+        <v>604.48</v>
+      </c>
+      <c r="F111">
+        <v>604.49</v>
+      </c>
+      <c r="G111">
+        <v>506.41</v>
+      </c>
+      <c r="H111">
+        <v>435.89</v>
+      </c>
+      <c r="I111">
+        <v>399.05</v>
+      </c>
+      <c r="J111">
+        <v>390.58</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>6600</v>
+      </c>
+      <c r="B112">
+        <v>985.05</v>
+      </c>
+      <c r="C112">
+        <v>923.1</v>
+      </c>
+      <c r="D112">
+        <v>759.48</v>
+      </c>
+      <c r="E112">
+        <v>608.16999999999996</v>
+      </c>
+      <c r="F112">
+        <v>608.19000000000005</v>
+      </c>
+      <c r="G112">
+        <v>510.35</v>
+      </c>
+      <c r="H112">
+        <v>439.94</v>
+      </c>
+      <c r="I112">
+        <v>403.12</v>
+      </c>
+      <c r="J112">
+        <v>394.64</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>6660</v>
+      </c>
+      <c r="B113">
+        <v>986.78</v>
+      </c>
+      <c r="C113">
+        <v>925.28</v>
+      </c>
+      <c r="D113">
+        <v>762.6</v>
+      </c>
+      <c r="E113">
+        <v>611.84</v>
+      </c>
+      <c r="F113">
+        <v>611.85</v>
+      </c>
+      <c r="G113">
+        <v>514.27</v>
+      </c>
+      <c r="H113">
+        <v>443.96</v>
+      </c>
+      <c r="I113">
+        <v>407.16</v>
+      </c>
+      <c r="J113">
+        <v>398.68</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>6720</v>
+      </c>
+      <c r="B114">
+        <v>988.48</v>
+      </c>
+      <c r="C114">
+        <v>927.44</v>
+      </c>
+      <c r="D114">
+        <v>765.68</v>
+      </c>
+      <c r="E114">
+        <v>615.48</v>
+      </c>
+      <c r="F114">
+        <v>615.49</v>
+      </c>
+      <c r="G114">
+        <v>518.15</v>
+      </c>
+      <c r="H114">
+        <v>447.96</v>
+      </c>
+      <c r="I114">
+        <v>411.19</v>
+      </c>
+      <c r="J114">
+        <v>402.7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>6780</v>
+      </c>
+      <c r="B115">
+        <v>990.17</v>
+      </c>
+      <c r="C115">
+        <v>929.57</v>
+      </c>
+      <c r="D115">
+        <v>768.74</v>
+      </c>
+      <c r="E115">
+        <v>619.09</v>
+      </c>
+      <c r="F115">
+        <v>619.1</v>
+      </c>
+      <c r="G115">
+        <v>522.01</v>
+      </c>
+      <c r="H115">
+        <v>451.93</v>
+      </c>
+      <c r="I115">
+        <v>415.2</v>
+      </c>
+      <c r="J115">
+        <v>406.7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>6840</v>
+      </c>
+      <c r="B116">
+        <v>991.84</v>
+      </c>
+      <c r="C116">
+        <v>931.67</v>
+      </c>
+      <c r="D116">
+        <v>771.77</v>
+      </c>
+      <c r="E116">
+        <v>622.66999999999996</v>
+      </c>
+      <c r="F116">
+        <v>622.67999999999995</v>
+      </c>
+      <c r="G116">
+        <v>525.84</v>
+      </c>
+      <c r="H116">
+        <v>455.87</v>
+      </c>
+      <c r="I116">
+        <v>419.18</v>
+      </c>
+      <c r="J116">
+        <v>410.69</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>6900</v>
+      </c>
+      <c r="B117">
+        <v>993.49</v>
+      </c>
+      <c r="C117">
+        <v>933.76</v>
+      </c>
+      <c r="D117">
+        <v>774.77</v>
+      </c>
+      <c r="E117">
+        <v>626.23</v>
+      </c>
+      <c r="F117">
+        <v>626.24</v>
+      </c>
+      <c r="G117">
+        <v>529.64</v>
+      </c>
+      <c r="H117">
+        <v>459.79</v>
+      </c>
+      <c r="I117">
+        <v>423.14</v>
+      </c>
+      <c r="J117">
+        <v>414.66</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>6960</v>
+      </c>
+      <c r="B118">
+        <v>995.12</v>
+      </c>
+      <c r="C118">
+        <v>935.82</v>
+      </c>
+      <c r="D118">
+        <v>777.75</v>
+      </c>
+      <c r="E118">
+        <v>629.75</v>
+      </c>
+      <c r="F118">
+        <v>629.76</v>
+      </c>
+      <c r="G118">
+        <v>533.41999999999996</v>
+      </c>
+      <c r="H118">
+        <v>463.69</v>
+      </c>
+      <c r="I118">
+        <v>427.08</v>
+      </c>
+      <c r="J118">
+        <v>418.6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>7020</v>
+      </c>
+      <c r="B119">
+        <v>996.73</v>
+      </c>
+      <c r="C119">
+        <v>937.86</v>
+      </c>
+      <c r="D119">
+        <v>780.7</v>
+      </c>
+      <c r="E119">
+        <v>633.25</v>
+      </c>
+      <c r="F119">
+        <v>633.26</v>
+      </c>
+      <c r="G119">
+        <v>537.16999999999996</v>
+      </c>
+      <c r="H119">
+        <v>467.56</v>
+      </c>
+      <c r="I119">
+        <v>431</v>
+      </c>
+      <c r="J119">
+        <v>422.53</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>7080</v>
+      </c>
+      <c r="B120">
+        <v>998.33</v>
+      </c>
+      <c r="C120">
+        <v>939.88</v>
+      </c>
+      <c r="D120">
+        <v>783.62</v>
+      </c>
+      <c r="E120">
+        <v>636.72</v>
+      </c>
+      <c r="F120">
+        <v>636.73</v>
+      </c>
+      <c r="G120">
+        <v>540.89</v>
+      </c>
+      <c r="H120">
+        <v>471.4</v>
+      </c>
+      <c r="I120">
+        <v>434.89</v>
+      </c>
+      <c r="J120">
+        <v>426.43</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>7140</v>
+      </c>
+      <c r="B121">
+        <v>999.91</v>
+      </c>
+      <c r="C121">
+        <v>941.87</v>
+      </c>
+      <c r="D121">
+        <v>786.51</v>
+      </c>
+      <c r="E121">
+        <v>640.16</v>
+      </c>
+      <c r="F121">
+        <v>640.16999999999996</v>
+      </c>
+      <c r="G121">
+        <v>544.59</v>
+      </c>
+      <c r="H121">
+        <v>475.23</v>
+      </c>
+      <c r="I121">
+        <v>438.77</v>
+      </c>
+      <c r="J121">
+        <v>430.32</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>7200</v>
+      </c>
+      <c r="B122">
+        <v>1001.5</v>
+      </c>
+      <c r="C122">
+        <v>943.85</v>
+      </c>
+      <c r="D122">
+        <v>789.39</v>
+      </c>
+      <c r="E122">
+        <v>643.58000000000004</v>
+      </c>
+      <c r="F122">
+        <v>643.59</v>
+      </c>
+      <c r="G122">
+        <v>548.26</v>
+      </c>
+      <c r="H122">
+        <v>479.03</v>
+      </c>
+      <c r="I122">
+        <v>442.62</v>
+      </c>
+      <c r="J122">
+        <v>434.18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>7260</v>
+      </c>
+      <c r="B123">
+        <v>1003</v>
+      </c>
+      <c r="C123">
+        <v>945.8</v>
+      </c>
+      <c r="D123">
+        <v>792.23</v>
+      </c>
+      <c r="E123">
+        <v>646.97</v>
+      </c>
+      <c r="F123">
+        <v>646.98</v>
+      </c>
+      <c r="G123">
+        <v>551.9</v>
+      </c>
+      <c r="H123">
+        <v>482.8</v>
+      </c>
+      <c r="I123">
+        <v>446.45</v>
+      </c>
+      <c r="J123">
+        <v>438.02</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>7320</v>
+      </c>
+      <c r="B124">
+        <v>1004.6</v>
+      </c>
+      <c r="C124">
+        <v>947.74</v>
+      </c>
+      <c r="D124">
+        <v>795.06</v>
+      </c>
+      <c r="E124">
+        <v>650.33000000000004</v>
+      </c>
+      <c r="F124">
+        <v>650.34</v>
+      </c>
+      <c r="G124">
+        <v>555.52</v>
+      </c>
+      <c r="H124">
+        <v>486.56</v>
+      </c>
+      <c r="I124">
+        <v>450.25</v>
+      </c>
+      <c r="J124">
+        <v>441.84</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>7380</v>
+      </c>
+      <c r="B125">
+        <v>1006.1</v>
+      </c>
+      <c r="C125">
+        <v>949.65</v>
+      </c>
+      <c r="D125">
+        <v>797.85</v>
+      </c>
+      <c r="E125">
+        <v>653.66999999999996</v>
+      </c>
+      <c r="F125">
+        <v>653.67999999999995</v>
+      </c>
+      <c r="G125">
+        <v>559.12</v>
+      </c>
+      <c r="H125">
+        <v>490.29</v>
+      </c>
+      <c r="I125">
+        <v>454.04</v>
+      </c>
+      <c r="J125">
+        <v>445.63</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>7440</v>
+      </c>
+      <c r="B126">
+        <v>1007.6</v>
+      </c>
+      <c r="C126">
+        <v>951.55</v>
+      </c>
+      <c r="D126">
+        <v>800.63</v>
+      </c>
+      <c r="E126">
+        <v>656.99</v>
+      </c>
+      <c r="F126">
+        <v>657</v>
+      </c>
+      <c r="G126">
+        <v>562.69000000000005</v>
+      </c>
+      <c r="H126">
+        <v>494</v>
+      </c>
+      <c r="I126">
+        <v>457.8</v>
+      </c>
+      <c r="J126">
+        <v>449.41</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>7500</v>
+      </c>
+      <c r="B127">
+        <v>1009.1</v>
+      </c>
+      <c r="C127">
+        <v>953.43</v>
+      </c>
+      <c r="D127">
+        <v>803.38</v>
+      </c>
+      <c r="E127">
+        <v>660.28</v>
+      </c>
+      <c r="F127">
+        <v>660.29</v>
+      </c>
+      <c r="G127">
+        <v>566.24</v>
+      </c>
+      <c r="H127">
+        <v>497.69</v>
+      </c>
+      <c r="I127">
+        <v>461.54</v>
+      </c>
+      <c r="J127">
+        <v>453.16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>7560</v>
+      </c>
+      <c r="B128">
+        <v>1010.5</v>
+      </c>
+      <c r="C128">
+        <v>955.29</v>
+      </c>
+      <c r="D128">
+        <v>806.11</v>
+      </c>
+      <c r="E128">
+        <v>663.54</v>
+      </c>
+      <c r="F128">
+        <v>663.55</v>
+      </c>
+      <c r="G128">
+        <v>569.77</v>
+      </c>
+      <c r="H128">
+        <v>501.36</v>
+      </c>
+      <c r="I128">
+        <v>465.26</v>
+      </c>
+      <c r="J128">
+        <v>456.89</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>7620</v>
+      </c>
+      <c r="B129">
+        <v>1012</v>
+      </c>
+      <c r="C129">
+        <v>957.13</v>
+      </c>
+      <c r="D129">
+        <v>808.81</v>
+      </c>
+      <c r="E129">
+        <v>666.78</v>
+      </c>
+      <c r="F129">
+        <v>666.79</v>
+      </c>
+      <c r="G129">
+        <v>573.27</v>
+      </c>
+      <c r="H129">
+        <v>505</v>
+      </c>
+      <c r="I129">
+        <v>468.95</v>
+      </c>
+      <c r="J129">
+        <v>460.6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>7680</v>
+      </c>
+      <c r="B130">
+        <v>1013.4</v>
+      </c>
+      <c r="C130">
+        <v>958.95</v>
+      </c>
+      <c r="D130">
+        <v>811.49</v>
+      </c>
+      <c r="E130">
+        <v>670</v>
+      </c>
+      <c r="F130">
+        <v>670.01</v>
+      </c>
+      <c r="G130">
+        <v>576.75</v>
+      </c>
+      <c r="H130">
+        <v>508.63</v>
+      </c>
+      <c r="I130">
+        <v>472.63</v>
+      </c>
+      <c r="J130">
+        <v>464.29</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>7740</v>
+      </c>
+      <c r="B131">
+        <v>1014.9</v>
+      </c>
+      <c r="C131">
+        <v>960.76</v>
+      </c>
+      <c r="D131">
+        <v>814.15</v>
+      </c>
+      <c r="E131">
+        <v>673.2</v>
+      </c>
+      <c r="F131">
+        <v>673.21</v>
+      </c>
+      <c r="G131">
+        <v>580.21</v>
+      </c>
+      <c r="H131">
+        <v>512.23</v>
+      </c>
+      <c r="I131">
+        <v>476.28</v>
+      </c>
+      <c r="J131">
+        <v>467.95</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>7800</v>
+      </c>
+      <c r="B132">
+        <v>1016.3</v>
+      </c>
+      <c r="C132">
+        <v>962.55</v>
+      </c>
+      <c r="D132">
+        <v>816.78</v>
+      </c>
+      <c r="E132">
+        <v>676.37</v>
+      </c>
+      <c r="F132">
+        <v>676.38</v>
+      </c>
+      <c r="G132">
+        <v>583.65</v>
+      </c>
+      <c r="H132">
+        <v>515.80999999999995</v>
+      </c>
+      <c r="I132">
+        <v>479.91</v>
+      </c>
+      <c r="J132">
+        <v>471.6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>7860</v>
+      </c>
+      <c r="B133">
+        <v>1017.7</v>
+      </c>
+      <c r="C133">
+        <v>964.32</v>
+      </c>
+      <c r="D133">
+        <v>819.39</v>
+      </c>
+      <c r="E133">
+        <v>679.52</v>
+      </c>
+      <c r="F133">
+        <v>679.53</v>
+      </c>
+      <c r="G133">
+        <v>587.05999999999995</v>
+      </c>
+      <c r="H133">
+        <v>519.36</v>
+      </c>
+      <c r="I133">
+        <v>483.53</v>
+      </c>
+      <c r="J133">
+        <v>475.22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>7920</v>
+      </c>
+      <c r="B134">
+        <v>1019.1</v>
+      </c>
+      <c r="C134">
+        <v>966.07</v>
+      </c>
+      <c r="D134">
+        <v>821.97</v>
+      </c>
+      <c r="E134">
+        <v>682.65</v>
+      </c>
+      <c r="F134">
+        <v>682.66</v>
+      </c>
+      <c r="G134">
+        <v>590.46</v>
+      </c>
+      <c r="H134">
+        <v>522.9</v>
+      </c>
+      <c r="I134">
+        <v>487.12</v>
+      </c>
+      <c r="J134">
+        <v>478.83</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>7980</v>
+      </c>
+      <c r="B135">
+        <v>1020.5</v>
+      </c>
+      <c r="C135">
+        <v>967.81</v>
+      </c>
+      <c r="D135">
+        <v>824.53</v>
+      </c>
+      <c r="E135">
+        <v>685.75</v>
+      </c>
+      <c r="F135">
+        <v>685.76</v>
+      </c>
+      <c r="G135">
+        <v>593.83000000000004</v>
+      </c>
+      <c r="H135">
+        <v>526.41</v>
+      </c>
+      <c r="I135">
+        <v>490.69</v>
+      </c>
+      <c r="J135">
+        <v>482.41</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>8040</v>
+      </c>
+      <c r="B136">
+        <v>1021.8</v>
+      </c>
+      <c r="C136">
+        <v>969.54</v>
+      </c>
+      <c r="D136">
+        <v>827.08</v>
+      </c>
+      <c r="E136">
+        <v>688.84</v>
+      </c>
+      <c r="F136">
+        <v>688.85</v>
+      </c>
+      <c r="G136">
+        <v>597.17999999999995</v>
+      </c>
+      <c r="H136">
+        <v>529.9</v>
+      </c>
+      <c r="I136">
+        <v>494.24</v>
+      </c>
+      <c r="J136">
+        <v>485.97</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>8100</v>
+      </c>
+      <c r="B137">
+        <v>1023.2</v>
+      </c>
+      <c r="C137">
+        <v>971.25</v>
+      </c>
+      <c r="D137">
+        <v>829.6</v>
+      </c>
+      <c r="E137">
+        <v>691.9</v>
+      </c>
+      <c r="F137">
+        <v>691.91</v>
+      </c>
+      <c r="G137">
+        <v>600.51</v>
+      </c>
+      <c r="H137">
+        <v>533.38</v>
+      </c>
+      <c r="I137">
+        <v>497.78</v>
+      </c>
+      <c r="J137">
+        <v>489.52</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>8160</v>
+      </c>
+      <c r="B138">
+        <v>1024.5</v>
+      </c>
+      <c r="C138">
+        <v>972.94</v>
+      </c>
+      <c r="D138">
+        <v>832.09</v>
+      </c>
+      <c r="E138">
+        <v>694.94</v>
+      </c>
+      <c r="F138">
+        <v>694.95</v>
+      </c>
+      <c r="G138">
+        <v>603.82000000000005</v>
+      </c>
+      <c r="H138">
+        <v>536.82000000000005</v>
+      </c>
+      <c r="I138">
+        <v>501.29</v>
+      </c>
+      <c r="J138">
+        <v>493.04</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>8220</v>
+      </c>
+      <c r="B139">
+        <v>1025.8</v>
+      </c>
+      <c r="C139">
+        <v>974.62</v>
+      </c>
+      <c r="D139">
+        <v>834.57</v>
+      </c>
+      <c r="E139">
+        <v>697.96</v>
+      </c>
+      <c r="F139">
+        <v>697.97</v>
+      </c>
+      <c r="G139">
+        <v>607.11</v>
+      </c>
+      <c r="H139">
+        <v>540.25</v>
+      </c>
+      <c r="I139">
+        <v>504.79</v>
+      </c>
+      <c r="J139">
+        <v>496.55</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>8280</v>
+      </c>
+      <c r="B140">
+        <v>1027.2</v>
+      </c>
+      <c r="C140">
+        <v>976.28</v>
+      </c>
+      <c r="D140">
+        <v>837.03</v>
+      </c>
+      <c r="E140">
+        <v>700.96</v>
+      </c>
+      <c r="F140">
+        <v>700.97</v>
+      </c>
+      <c r="G140">
+        <v>610.37</v>
+      </c>
+      <c r="H140">
+        <v>543.66</v>
+      </c>
+      <c r="I140">
+        <v>508.26</v>
+      </c>
+      <c r="J140">
+        <v>500.03</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>8340</v>
+      </c>
+      <c r="B141">
+        <v>1028.5</v>
+      </c>
+      <c r="C141">
+        <v>977.93</v>
+      </c>
+      <c r="D141">
+        <v>839.47</v>
+      </c>
+      <c r="E141">
+        <v>703.94</v>
+      </c>
+      <c r="F141">
+        <v>703.95</v>
+      </c>
+      <c r="G141">
+        <v>613.62</v>
+      </c>
+      <c r="H141">
+        <v>547.04999999999995</v>
+      </c>
+      <c r="I141">
+        <v>511.72</v>
+      </c>
+      <c r="J141">
+        <v>503.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>8400</v>
+      </c>
+      <c r="B142">
+        <v>1029.8</v>
+      </c>
+      <c r="C142">
+        <v>979.57</v>
+      </c>
+      <c r="D142">
+        <v>841.88</v>
+      </c>
+      <c r="E142">
+        <v>706.9</v>
+      </c>
+      <c r="F142">
+        <v>706.91</v>
+      </c>
+      <c r="G142">
+        <v>616.84</v>
+      </c>
+      <c r="H142">
+        <v>550.41999999999996</v>
+      </c>
+      <c r="I142">
+        <v>515.16</v>
+      </c>
+      <c r="J142">
+        <v>506.95</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>8460</v>
+      </c>
+      <c r="B143">
+        <v>1031</v>
+      </c>
+      <c r="C143">
+        <v>981.19</v>
+      </c>
+      <c r="D143">
+        <v>844.28</v>
+      </c>
+      <c r="E143">
+        <v>709.84</v>
+      </c>
+      <c r="F143">
+        <v>709.85</v>
+      </c>
+      <c r="G143">
+        <v>620.04999999999995</v>
+      </c>
+      <c r="H143">
+        <v>553.77</v>
+      </c>
+      <c r="I143">
+        <v>518.57000000000005</v>
+      </c>
+      <c r="J143">
+        <v>510.38</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>8520</v>
+      </c>
+      <c r="B144">
+        <v>1032.3</v>
+      </c>
+      <c r="C144">
+        <v>982.79</v>
+      </c>
+      <c r="D144">
+        <v>846.66</v>
+      </c>
+      <c r="E144">
+        <v>712.76</v>
+      </c>
+      <c r="F144">
+        <v>712.77</v>
+      </c>
+      <c r="G144">
+        <v>623.23</v>
+      </c>
+      <c r="H144">
+        <v>557.09</v>
+      </c>
+      <c r="I144">
+        <v>521.97</v>
+      </c>
+      <c r="J144">
+        <v>513.79999999999995</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>8580</v>
+      </c>
+      <c r="B145">
+        <v>1033.5999999999999</v>
+      </c>
+      <c r="C145">
+        <v>984.39</v>
+      </c>
+      <c r="D145">
+        <v>849.02</v>
+      </c>
+      <c r="E145">
+        <v>715.66</v>
+      </c>
+      <c r="F145">
+        <v>715.67</v>
+      </c>
+      <c r="G145">
+        <v>626.4</v>
+      </c>
+      <c r="H145">
+        <v>560.4</v>
+      </c>
+      <c r="I145">
+        <v>525.35</v>
+      </c>
+      <c r="J145">
+        <v>517.19000000000005</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>8640</v>
+      </c>
+      <c r="B146">
+        <v>1034.8</v>
+      </c>
+      <c r="C146">
+        <v>985.97</v>
+      </c>
+      <c r="D146">
+        <v>851.36</v>
+      </c>
+      <c r="E146">
+        <v>718.54</v>
+      </c>
+      <c r="F146">
+        <v>718.55</v>
+      </c>
+      <c r="G146">
+        <v>629.54</v>
+      </c>
+      <c r="H146">
+        <v>563.69000000000005</v>
+      </c>
+      <c r="I146">
+        <v>528.71</v>
+      </c>
+      <c r="J146">
+        <v>520.57000000000005</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>8700</v>
+      </c>
+      <c r="B147">
+        <v>1036.0999999999999</v>
+      </c>
+      <c r="C147">
+        <v>987.53</v>
+      </c>
+      <c r="D147">
+        <v>853.68</v>
+      </c>
+      <c r="E147">
+        <v>721.4</v>
+      </c>
+      <c r="F147">
+        <v>721.41</v>
+      </c>
+      <c r="G147">
+        <v>632.66</v>
+      </c>
+      <c r="H147">
+        <v>566.97</v>
+      </c>
+      <c r="I147">
+        <v>532.04999999999995</v>
+      </c>
+      <c r="J147">
+        <v>523.91999999999996</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>8760</v>
+      </c>
+      <c r="B148">
+        <v>1037.3</v>
+      </c>
+      <c r="C148">
+        <v>989.09</v>
+      </c>
+      <c r="D148">
+        <v>855.98</v>
+      </c>
+      <c r="E148">
+        <v>724.24</v>
+      </c>
+      <c r="F148">
+        <v>724.25</v>
+      </c>
+      <c r="G148">
+        <v>635.77</v>
+      </c>
+      <c r="H148">
+        <v>570.22</v>
+      </c>
+      <c r="I148">
+        <v>535.38</v>
+      </c>
+      <c r="J148">
+        <v>527.26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>8820</v>
+      </c>
+      <c r="B149">
+        <v>1038.5</v>
+      </c>
+      <c r="C149">
+        <v>990.63</v>
+      </c>
+      <c r="D149">
+        <v>858.27</v>
+      </c>
+      <c r="E149">
+        <v>727.05</v>
+      </c>
+      <c r="F149">
+        <v>727.06</v>
+      </c>
+      <c r="G149">
+        <v>638.85</v>
+      </c>
+      <c r="H149">
+        <v>573.45000000000005</v>
+      </c>
+      <c r="I149">
+        <v>538.67999999999995</v>
+      </c>
+      <c r="J149">
+        <v>530.58000000000004</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>8880</v>
+      </c>
+      <c r="B150">
+        <v>1039.7</v>
+      </c>
+      <c r="C150">
+        <v>992.16</v>
+      </c>
+      <c r="D150">
+        <v>860.53</v>
+      </c>
+      <c r="E150">
+        <v>729.85</v>
+      </c>
+      <c r="F150">
+        <v>729.86</v>
+      </c>
+      <c r="G150">
+        <v>641.91999999999996</v>
+      </c>
+      <c r="H150">
+        <v>576.66999999999996</v>
+      </c>
+      <c r="I150">
+        <v>541.96</v>
+      </c>
+      <c r="J150">
+        <v>533.88</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>8940</v>
+      </c>
+      <c r="B151">
+        <v>1040.9000000000001</v>
+      </c>
+      <c r="C151">
+        <v>993.67</v>
+      </c>
+      <c r="D151">
+        <v>862.78</v>
+      </c>
+      <c r="E151">
+        <v>732.63</v>
+      </c>
+      <c r="F151">
+        <v>732.64</v>
+      </c>
+      <c r="G151">
+        <v>644.96</v>
+      </c>
+      <c r="H151">
+        <v>579.87</v>
+      </c>
+      <c r="I151">
+        <v>545.23</v>
+      </c>
+      <c r="J151">
+        <v>537.16999999999996</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>9000</v>
+      </c>
+      <c r="B152">
+        <v>1042.0999999999999</v>
+      </c>
+      <c r="C152">
+        <v>995.18</v>
+      </c>
+      <c r="D152">
+        <v>865.02</v>
+      </c>
+      <c r="E152">
+        <v>735.39</v>
+      </c>
+      <c r="F152">
+        <v>735.4</v>
+      </c>
+      <c r="G152">
+        <v>647.99</v>
+      </c>
+      <c r="H152">
+        <v>583.04999999999995</v>
+      </c>
+      <c r="I152">
+        <v>548.48</v>
+      </c>
+      <c r="J152">
+        <v>540.42999999999995</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>9060</v>
+      </c>
+      <c r="B153">
+        <v>1043.3</v>
+      </c>
+      <c r="C153">
+        <v>996.67</v>
+      </c>
+      <c r="D153">
+        <v>867.23</v>
+      </c>
+      <c r="E153">
+        <v>738.14</v>
+      </c>
+      <c r="F153">
+        <v>738.15</v>
+      </c>
+      <c r="G153">
+        <v>651</v>
+      </c>
+      <c r="H153">
+        <v>586.21</v>
+      </c>
+      <c r="I153">
+        <v>551.71</v>
+      </c>
+      <c r="J153">
+        <v>543.67999999999995</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>9120</v>
+      </c>
+      <c r="B154">
+        <v>1044.5</v>
+      </c>
+      <c r="C154">
+        <v>998.15</v>
+      </c>
+      <c r="D154">
+        <v>869.43</v>
+      </c>
+      <c r="E154">
+        <v>740.86</v>
+      </c>
+      <c r="F154">
+        <v>740.87</v>
+      </c>
+      <c r="G154">
+        <v>653.99</v>
+      </c>
+      <c r="H154">
+        <v>589.36</v>
+      </c>
+      <c r="I154">
+        <v>554.91999999999996</v>
+      </c>
+      <c r="J154">
+        <v>546.91</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>9180</v>
+      </c>
+      <c r="B155">
+        <v>1045.5999999999999</v>
+      </c>
+      <c r="C155">
+        <v>999.61</v>
+      </c>
+      <c r="D155">
+        <v>871.61</v>
+      </c>
+      <c r="E155">
+        <v>743.56</v>
+      </c>
+      <c r="F155">
+        <v>743.58</v>
+      </c>
+      <c r="G155">
+        <v>656.96</v>
+      </c>
+      <c r="H155">
+        <v>592.49</v>
+      </c>
+      <c r="I155">
+        <v>558.12</v>
+      </c>
+      <c r="J155">
+        <v>550.12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>9240</v>
+      </c>
+      <c r="B156">
+        <v>1046.8</v>
+      </c>
+      <c r="C156">
+        <v>1001.1</v>
+      </c>
+      <c r="D156">
+        <v>873.78</v>
+      </c>
+      <c r="E156">
+        <v>746.25</v>
+      </c>
+      <c r="F156">
+        <v>746.26</v>
+      </c>
+      <c r="G156">
+        <v>659.92</v>
+      </c>
+      <c r="H156">
+        <v>595.6</v>
+      </c>
+      <c r="I156">
+        <v>561.29</v>
+      </c>
+      <c r="J156">
+        <v>553.30999999999995</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>9300</v>
+      </c>
+      <c r="B157">
+        <v>1047.9000000000001</v>
+      </c>
+      <c r="C157">
+        <v>1002.5</v>
+      </c>
+      <c r="D157">
+        <v>875.93</v>
+      </c>
+      <c r="E157">
+        <v>748.92</v>
+      </c>
+      <c r="F157">
+        <v>748.93</v>
+      </c>
+      <c r="G157">
+        <v>662.85</v>
+      </c>
+      <c r="H157">
+        <v>598.69000000000005</v>
+      </c>
+      <c r="I157">
+        <v>564.45000000000005</v>
+      </c>
+      <c r="J157">
+        <v>556.48</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>9360</v>
+      </c>
+      <c r="B158">
+        <v>1049.0999999999999</v>
+      </c>
+      <c r="C158">
+        <v>1003.9</v>
+      </c>
+      <c r="D158">
+        <v>878.07</v>
+      </c>
+      <c r="E158">
+        <v>751.57</v>
+      </c>
+      <c r="F158">
+        <v>751.58</v>
+      </c>
+      <c r="G158">
+        <v>665.77</v>
+      </c>
+      <c r="H158">
+        <v>601.77</v>
+      </c>
+      <c r="I158">
+        <v>567.59</v>
+      </c>
+      <c r="J158">
+        <v>559.64</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>9420</v>
+      </c>
+      <c r="B159">
+        <v>1050.2</v>
+      </c>
+      <c r="C159">
+        <v>1005.4</v>
+      </c>
+      <c r="D159">
+        <v>880.18</v>
+      </c>
+      <c r="E159">
+        <v>754.21</v>
+      </c>
+      <c r="F159">
+        <v>754.22</v>
+      </c>
+      <c r="G159">
+        <v>668.68</v>
+      </c>
+      <c r="H159">
+        <v>604.83000000000004</v>
+      </c>
+      <c r="I159">
+        <v>570.72</v>
+      </c>
+      <c r="J159">
+        <v>562.78</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>9480</v>
+      </c>
+      <c r="B160">
+        <v>1051.3</v>
+      </c>
+      <c r="C160">
+        <v>1006.8</v>
+      </c>
+      <c r="D160">
+        <v>882.29</v>
+      </c>
+      <c r="E160">
+        <v>756.82</v>
+      </c>
+      <c r="F160">
+        <v>756.83</v>
+      </c>
+      <c r="G160">
+        <v>671.56</v>
+      </c>
+      <c r="H160">
+        <v>607.88</v>
+      </c>
+      <c r="I160">
+        <v>573.83000000000004</v>
+      </c>
+      <c r="J160">
+        <v>565.91</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>9540</v>
+      </c>
+      <c r="B161">
+        <v>1052.4000000000001</v>
+      </c>
+      <c r="C161">
+        <v>1008.2</v>
+      </c>
+      <c r="D161">
+        <v>884.38</v>
+      </c>
+      <c r="E161">
+        <v>759.42</v>
+      </c>
+      <c r="F161">
+        <v>759.43</v>
+      </c>
+      <c r="G161">
+        <v>674.43</v>
+      </c>
+      <c r="H161">
+        <v>610.9</v>
+      </c>
+      <c r="I161">
+        <v>576.91999999999996</v>
+      </c>
+      <c r="J161">
+        <v>569.01</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>9600</v>
+      </c>
+      <c r="B162">
+        <v>1053.5</v>
+      </c>
+      <c r="C162">
+        <v>1009.6</v>
+      </c>
+      <c r="D162">
+        <v>886.45</v>
+      </c>
+      <c r="E162">
+        <v>762.01</v>
+      </c>
+      <c r="F162">
+        <v>762.02</v>
+      </c>
+      <c r="G162">
+        <v>677.28</v>
+      </c>
+      <c r="H162">
+        <v>613.91</v>
+      </c>
+      <c r="I162">
+        <v>579.99</v>
+      </c>
+      <c r="J162">
+        <v>572.1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>9660</v>
+      </c>
+      <c r="B163">
+        <v>1054.5999999999999</v>
+      </c>
+      <c r="C163">
+        <v>1010.9</v>
+      </c>
+      <c r="D163">
+        <v>888.51</v>
+      </c>
+      <c r="E163">
+        <v>764.57</v>
+      </c>
+      <c r="F163">
+        <v>764.58</v>
+      </c>
+      <c r="G163">
+        <v>680.12</v>
+      </c>
+      <c r="H163">
+        <v>616.91</v>
+      </c>
+      <c r="I163">
+        <v>583.04999999999995</v>
+      </c>
+      <c r="J163">
+        <v>575.16999999999996</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>9720</v>
+      </c>
+      <c r="B164">
+        <v>1055.7</v>
+      </c>
+      <c r="C164">
+        <v>1012.3</v>
+      </c>
+      <c r="D164">
+        <v>890.55</v>
+      </c>
+      <c r="E164">
+        <v>767.12</v>
+      </c>
+      <c r="F164">
+        <v>767.13</v>
+      </c>
+      <c r="G164">
+        <v>682.94</v>
+      </c>
+      <c r="H164">
+        <v>619.89</v>
+      </c>
+      <c r="I164">
+        <v>586.1</v>
+      </c>
+      <c r="J164">
+        <v>578.23</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>9780</v>
+      </c>
+      <c r="B165">
+        <v>1056.8</v>
+      </c>
+      <c r="C165">
+        <v>1013.7</v>
+      </c>
+      <c r="D165">
+        <v>892.58</v>
+      </c>
+      <c r="E165">
+        <v>769.66</v>
+      </c>
+      <c r="F165">
+        <v>769.67</v>
+      </c>
+      <c r="G165">
+        <v>685.75</v>
+      </c>
+      <c r="H165">
+        <v>622.85</v>
+      </c>
+      <c r="I165">
+        <v>589.12</v>
+      </c>
+      <c r="J165">
+        <v>581.27</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>9840</v>
+      </c>
+      <c r="B166">
+        <v>1057.9000000000001</v>
+      </c>
+      <c r="C166">
+        <v>1015</v>
+      </c>
+      <c r="D166">
+        <v>894.6</v>
+      </c>
+      <c r="E166">
+        <v>772.18</v>
+      </c>
+      <c r="F166">
+        <v>772.19</v>
+      </c>
+      <c r="G166">
+        <v>688.53</v>
+      </c>
+      <c r="H166">
+        <v>625.79</v>
+      </c>
+      <c r="I166">
+        <v>592.14</v>
+      </c>
+      <c r="J166">
+        <v>584.29999999999995</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>9900</v>
+      </c>
+      <c r="B167">
+        <v>1058.9000000000001</v>
+      </c>
+      <c r="C167">
+        <v>1016.3</v>
+      </c>
+      <c r="D167">
+        <v>896.6</v>
+      </c>
+      <c r="E167">
+        <v>774.68</v>
+      </c>
+      <c r="F167">
+        <v>774.69</v>
+      </c>
+      <c r="G167">
+        <v>691.31</v>
+      </c>
+      <c r="H167">
+        <v>628.72</v>
+      </c>
+      <c r="I167">
+        <v>595.13</v>
+      </c>
+      <c r="J167">
+        <v>587.30999999999995</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>9960</v>
+      </c>
+      <c r="B168">
+        <v>1060</v>
+      </c>
+      <c r="C168">
+        <v>1017.7</v>
+      </c>
+      <c r="D168">
+        <v>898.58</v>
+      </c>
+      <c r="E168">
+        <v>777.17</v>
+      </c>
+      <c r="F168">
+        <v>777.18</v>
+      </c>
+      <c r="G168">
+        <v>694.06</v>
+      </c>
+      <c r="H168">
+        <v>631.63</v>
+      </c>
+      <c r="I168">
+        <v>598.11</v>
+      </c>
+      <c r="J168">
+        <v>590.29999999999995</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>10020</v>
+      </c>
+      <c r="B169">
+        <v>1061</v>
+      </c>
+      <c r="C169">
+        <v>1019</v>
+      </c>
+      <c r="D169">
+        <v>900.56</v>
+      </c>
+      <c r="E169">
+        <v>779.64</v>
+      </c>
+      <c r="F169">
+        <v>779.65</v>
+      </c>
+      <c r="G169">
+        <v>696.81</v>
+      </c>
+      <c r="H169">
+        <v>634.52</v>
+      </c>
+      <c r="I169">
+        <v>601.08000000000004</v>
+      </c>
+      <c r="J169">
+        <v>593.28</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>10080</v>
+      </c>
+      <c r="B170">
+        <v>1062.0999999999999</v>
+      </c>
+      <c r="C170">
+        <v>1020.3</v>
+      </c>
+      <c r="D170">
+        <v>902.51</v>
+      </c>
+      <c r="E170">
+        <v>782.09</v>
+      </c>
+      <c r="F170">
+        <v>782.1</v>
+      </c>
+      <c r="G170">
+        <v>699.53</v>
+      </c>
+      <c r="H170">
+        <v>637.4</v>
+      </c>
+      <c r="I170">
+        <v>604.03</v>
+      </c>
+      <c r="J170">
+        <v>596.24</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>10140</v>
+      </c>
+      <c r="B171">
+        <v>1063.0999999999999</v>
+      </c>
+      <c r="C171">
+        <v>1021.6</v>
+      </c>
+      <c r="D171">
+        <v>904.46</v>
+      </c>
+      <c r="E171">
+        <v>784.53</v>
+      </c>
+      <c r="F171">
+        <v>784.54</v>
+      </c>
+      <c r="G171">
+        <v>702.24</v>
+      </c>
+      <c r="H171">
+        <v>640.26</v>
+      </c>
+      <c r="I171">
+        <v>606.97</v>
+      </c>
+      <c r="J171">
+        <v>599.19000000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>10200</v>
+      </c>
+      <c r="B172">
+        <v>1064.0999999999999</v>
+      </c>
+      <c r="C172">
+        <v>1022.9</v>
+      </c>
+      <c r="D172">
+        <v>906.39</v>
+      </c>
+      <c r="E172">
+        <v>786.96</v>
+      </c>
+      <c r="F172">
+        <v>786.97</v>
+      </c>
+      <c r="G172">
+        <v>704.94</v>
+      </c>
+      <c r="H172">
+        <v>643.11</v>
+      </c>
+      <c r="I172">
+        <v>609.89</v>
+      </c>
+      <c r="J172">
+        <v>602.13</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>10260</v>
+      </c>
+      <c r="B173">
+        <v>1065.2</v>
+      </c>
+      <c r="C173">
+        <v>1024.0999999999999</v>
+      </c>
+      <c r="D173">
+        <v>908.3</v>
+      </c>
+      <c r="E173">
+        <v>789.37</v>
+      </c>
+      <c r="F173">
+        <v>789.38</v>
+      </c>
+      <c r="G173">
+        <v>707.62</v>
+      </c>
+      <c r="H173">
+        <v>645.94000000000005</v>
+      </c>
+      <c r="I173">
+        <v>612.79999999999995</v>
+      </c>
+      <c r="J173">
+        <v>605.04999999999995</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>10320</v>
+      </c>
+      <c r="B174">
+        <v>1066.2</v>
+      </c>
+      <c r="C174">
+        <v>1025.4000000000001</v>
+      </c>
+      <c r="D174">
+        <v>910.2</v>
+      </c>
+      <c r="E174">
+        <v>791.77</v>
+      </c>
+      <c r="F174">
+        <v>791.78</v>
+      </c>
+      <c r="G174">
+        <v>710.29</v>
+      </c>
+      <c r="H174">
+        <v>648.76</v>
+      </c>
+      <c r="I174">
+        <v>615.69000000000005</v>
+      </c>
+      <c r="J174">
+        <v>607.96</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>10380</v>
+      </c>
+      <c r="B175">
+        <v>1067.2</v>
+      </c>
+      <c r="C175">
+        <v>1026.7</v>
+      </c>
+      <c r="D175">
+        <v>912.09</v>
+      </c>
+      <c r="E175">
+        <v>794.15</v>
+      </c>
+      <c r="F175">
+        <v>794.16</v>
+      </c>
+      <c r="G175">
+        <v>712.94</v>
+      </c>
+      <c r="H175">
+        <v>651.55999999999995</v>
+      </c>
+      <c r="I175">
+        <v>618.55999999999995</v>
+      </c>
+      <c r="J175">
+        <v>610.85</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>10440</v>
+      </c>
+      <c r="B176">
+        <v>1068.2</v>
+      </c>
+      <c r="C176">
+        <v>1027.9000000000001</v>
+      </c>
+      <c r="D176">
+        <v>913.97</v>
+      </c>
+      <c r="E176">
+        <v>796.52</v>
+      </c>
+      <c r="F176">
+        <v>796.53</v>
+      </c>
+      <c r="G176">
+        <v>715.57</v>
+      </c>
+      <c r="H176">
+        <v>654.35</v>
+      </c>
+      <c r="I176">
+        <v>621.42999999999995</v>
+      </c>
+      <c r="J176">
+        <v>613.73</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>10500</v>
+      </c>
+      <c r="B177">
+        <v>1069.2</v>
+      </c>
+      <c r="C177">
+        <v>1029.2</v>
+      </c>
+      <c r="D177">
+        <v>915.83</v>
+      </c>
+      <c r="E177">
+        <v>798.87</v>
+      </c>
+      <c r="F177">
+        <v>798.88</v>
+      </c>
+      <c r="G177">
+        <v>718.19</v>
+      </c>
+      <c r="H177">
+        <v>657.12</v>
+      </c>
+      <c r="I177">
+        <v>624.27</v>
+      </c>
+      <c r="J177">
+        <v>616.59</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>10560</v>
+      </c>
+      <c r="B178">
+        <v>1070.2</v>
+      </c>
+      <c r="C178">
+        <v>1030.4000000000001</v>
+      </c>
+      <c r="D178">
+        <v>917.68</v>
+      </c>
+      <c r="E178">
+        <v>801.21</v>
+      </c>
+      <c r="F178">
+        <v>801.22</v>
+      </c>
+      <c r="G178">
+        <v>720.8</v>
+      </c>
+      <c r="H178">
+        <v>659.88</v>
+      </c>
+      <c r="I178">
+        <v>627.11</v>
+      </c>
+      <c r="J178">
+        <v>619.44000000000005</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>10620</v>
+      </c>
+      <c r="B179">
+        <v>1071.0999999999999</v>
+      </c>
+      <c r="C179">
+        <v>1031.5999999999999</v>
+      </c>
+      <c r="D179">
+        <v>919.51</v>
+      </c>
+      <c r="E179">
+        <v>803.54</v>
+      </c>
+      <c r="F179">
+        <v>803.55</v>
+      </c>
+      <c r="G179">
+        <v>723.38</v>
+      </c>
+      <c r="H179">
+        <v>662.62</v>
+      </c>
+      <c r="I179">
+        <v>629.92999999999995</v>
+      </c>
+      <c r="J179">
+        <v>622.28</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>10680</v>
+      </c>
+      <c r="B180">
+        <v>1072.0999999999999</v>
+      </c>
+      <c r="C180">
+        <v>1032.8</v>
+      </c>
+      <c r="D180">
+        <v>921.33</v>
+      </c>
+      <c r="E180">
+        <v>805.85</v>
+      </c>
+      <c r="F180">
+        <v>805.86</v>
+      </c>
+      <c r="G180">
+        <v>725.96</v>
+      </c>
+      <c r="H180">
+        <v>665.35</v>
+      </c>
+      <c r="I180">
+        <v>632.73</v>
+      </c>
+      <c r="J180">
+        <v>625.1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>10740</v>
+      </c>
+      <c r="B181">
+        <v>1073.0999999999999</v>
+      </c>
+      <c r="C181">
+        <v>1034</v>
+      </c>
+      <c r="D181">
+        <v>923.14</v>
+      </c>
+      <c r="E181">
+        <v>808.15</v>
+      </c>
+      <c r="F181">
+        <v>808.16</v>
+      </c>
+      <c r="G181">
+        <v>728.52</v>
+      </c>
+      <c r="H181">
+        <v>668.06</v>
+      </c>
+      <c r="I181">
+        <v>635.52</v>
+      </c>
+      <c r="J181">
+        <v>627.91</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>10800</v>
+      </c>
+      <c r="B182">
+        <v>1074</v>
+      </c>
+      <c r="C182">
+        <v>1035.2</v>
+      </c>
+      <c r="D182">
+        <v>924.94</v>
+      </c>
+      <c r="E182">
+        <v>810.44</v>
+      </c>
+      <c r="F182">
+        <v>810.45</v>
+      </c>
+      <c r="G182">
+        <v>731.06</v>
+      </c>
+      <c r="H182">
+        <v>670.76</v>
+      </c>
+      <c r="I182">
+        <v>638.29</v>
+      </c>
+      <c r="J182">
+        <v>630.70000000000005</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>10860</v>
+      </c>
+      <c r="B183">
+        <v>1075</v>
+      </c>
+      <c r="C183">
+        <v>1036.4000000000001</v>
+      </c>
+      <c r="D183">
+        <v>926.72</v>
+      </c>
+      <c r="E183">
+        <v>812.71</v>
+      </c>
+      <c r="F183">
+        <v>812.72</v>
+      </c>
+      <c r="G183">
+        <v>733.59</v>
+      </c>
+      <c r="H183">
+        <v>673.45</v>
+      </c>
+      <c r="I183">
+        <v>641.05999999999995</v>
+      </c>
+      <c r="J183">
+        <v>633.48</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>10920</v>
+      </c>
+      <c r="B184">
+        <v>1075.9000000000001</v>
+      </c>
+      <c r="C184">
+        <v>1037.5999999999999</v>
+      </c>
+      <c r="D184">
+        <v>928.49</v>
+      </c>
+      <c r="E184">
+        <v>814.96</v>
+      </c>
+      <c r="F184">
+        <v>814.97</v>
+      </c>
+      <c r="G184">
+        <v>736.11</v>
+      </c>
+      <c r="H184">
+        <v>676.12</v>
+      </c>
+      <c r="I184">
+        <v>643.79999999999995</v>
+      </c>
+      <c r="J184">
+        <v>636.24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>10980</v>
+      </c>
+      <c r="B185">
+        <v>1076.9000000000001</v>
+      </c>
+      <c r="C185">
+        <v>1038.8</v>
+      </c>
+      <c r="D185">
+        <v>930.25</v>
+      </c>
+      <c r="E185">
+        <v>817.2</v>
+      </c>
+      <c r="F185">
+        <v>817.21</v>
+      </c>
+      <c r="G185">
+        <v>738.61</v>
+      </c>
+      <c r="H185">
+        <v>678.78</v>
+      </c>
+      <c r="I185">
+        <v>646.53</v>
+      </c>
+      <c r="J185">
+        <v>638.99</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>11040</v>
+      </c>
+      <c r="B186">
+        <v>1077.8</v>
+      </c>
+      <c r="C186">
+        <v>1039.9000000000001</v>
+      </c>
+      <c r="D186">
+        <v>932</v>
+      </c>
+      <c r="E186">
+        <v>819.43</v>
+      </c>
+      <c r="F186">
+        <v>819.44</v>
+      </c>
+      <c r="G186">
+        <v>741.09</v>
+      </c>
+      <c r="H186">
+        <v>681.43</v>
+      </c>
+      <c r="I186">
+        <v>649.25</v>
+      </c>
+      <c r="J186">
+        <v>641.73</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>11100</v>
+      </c>
+      <c r="B187">
+        <v>1078.7</v>
+      </c>
+      <c r="C187">
+        <v>1041.0999999999999</v>
+      </c>
+      <c r="D187">
+        <v>933.74</v>
+      </c>
+      <c r="E187">
+        <v>821.65</v>
+      </c>
+      <c r="F187">
+        <v>821.65</v>
+      </c>
+      <c r="G187">
+        <v>743.57</v>
+      </c>
+      <c r="H187">
+        <v>684.06</v>
+      </c>
+      <c r="I187">
+        <v>651.96</v>
+      </c>
+      <c r="J187">
+        <v>644.45000000000005</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>11160</v>
+      </c>
+      <c r="B188">
+        <v>1079.7</v>
+      </c>
+      <c r="C188">
+        <v>1042.2</v>
+      </c>
+      <c r="D188">
+        <v>935.46</v>
+      </c>
+      <c r="E188">
+        <v>823.85</v>
+      </c>
+      <c r="F188">
+        <v>823.85</v>
+      </c>
+      <c r="G188">
+        <v>746.03</v>
+      </c>
+      <c r="H188">
+        <v>686.68</v>
+      </c>
+      <c r="I188">
+        <v>654.65</v>
+      </c>
+      <c r="J188">
+        <v>647.16</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>11220</v>
+      </c>
+      <c r="B189">
+        <v>1080.5999999999999</v>
+      </c>
+      <c r="C189">
+        <v>1043.4000000000001</v>
+      </c>
+      <c r="D189">
+        <v>937.17</v>
+      </c>
+      <c r="E189">
+        <v>826.03</v>
+      </c>
+      <c r="F189">
+        <v>826.04</v>
+      </c>
+      <c r="G189">
+        <v>748.47</v>
+      </c>
+      <c r="H189">
+        <v>689.29</v>
+      </c>
+      <c r="I189">
+        <v>657.33</v>
+      </c>
+      <c r="J189">
+        <v>649.85</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>11280</v>
+      </c>
+      <c r="B190">
+        <v>1081.5</v>
+      </c>
+      <c r="C190">
+        <v>1044.5</v>
+      </c>
+      <c r="D190">
+        <v>938.87</v>
+      </c>
+      <c r="E190">
+        <v>828.21</v>
+      </c>
+      <c r="F190">
+        <v>828.22</v>
+      </c>
+      <c r="G190">
+        <v>750.91</v>
+      </c>
+      <c r="H190">
+        <v>691.88</v>
+      </c>
+      <c r="I190">
+        <v>659.99</v>
+      </c>
+      <c r="J190">
+        <v>652.53</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>11340</v>
+      </c>
+      <c r="B191">
+        <v>1082.4000000000001</v>
+      </c>
+      <c r="C191">
+        <v>1045.5999999999999</v>
+      </c>
+      <c r="D191">
+        <v>940.56</v>
+      </c>
+      <c r="E191">
+        <v>830.37</v>
+      </c>
+      <c r="F191">
+        <v>830.38</v>
+      </c>
+      <c r="G191">
+        <v>753.32</v>
+      </c>
+      <c r="H191">
+        <v>694.46</v>
+      </c>
+      <c r="I191">
+        <v>662.64</v>
+      </c>
+      <c r="J191">
+        <v>655.20000000000005</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>11400</v>
+      </c>
+      <c r="B192">
+        <v>1083.3</v>
+      </c>
+      <c r="C192">
+        <v>1046.7</v>
+      </c>
+      <c r="D192">
+        <v>942.24</v>
+      </c>
+      <c r="E192">
+        <v>832.51</v>
+      </c>
+      <c r="F192">
+        <v>832.52</v>
+      </c>
+      <c r="G192">
+        <v>755.73</v>
+      </c>
+      <c r="H192">
+        <v>697.03</v>
+      </c>
+      <c r="I192">
+        <v>665.28</v>
+      </c>
+      <c r="J192">
+        <v>657.86</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>11460</v>
+      </c>
+      <c r="B193">
+        <v>1084.2</v>
+      </c>
+      <c r="C193">
+        <v>1047.8</v>
+      </c>
+      <c r="D193">
+        <v>943.91</v>
+      </c>
+      <c r="E193">
+        <v>834.65</v>
+      </c>
+      <c r="F193">
+        <v>834.66</v>
+      </c>
+      <c r="G193">
+        <v>758.12</v>
+      </c>
+      <c r="H193">
+        <v>699.59</v>
+      </c>
+      <c r="I193">
+        <v>667.91</v>
+      </c>
+      <c r="J193">
+        <v>660.5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>11520</v>
+      </c>
+      <c r="B194">
+        <v>1085.0999999999999</v>
+      </c>
+      <c r="C194">
+        <v>1048.9000000000001</v>
+      </c>
+      <c r="D194">
+        <v>945.56</v>
+      </c>
+      <c r="E194">
+        <v>836.77</v>
+      </c>
+      <c r="F194">
+        <v>836.78</v>
+      </c>
+      <c r="G194">
+        <v>760.5</v>
+      </c>
+      <c r="H194">
+        <v>702.13</v>
+      </c>
+      <c r="I194">
+        <v>670.52</v>
+      </c>
+      <c r="J194">
+        <v>663.13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>11580</v>
+      </c>
+      <c r="B195">
+        <v>1086</v>
+      </c>
+      <c r="C195">
+        <v>1050</v>
+      </c>
+      <c r="D195">
+        <v>947.21</v>
+      </c>
+      <c r="E195">
+        <v>838.88</v>
+      </c>
+      <c r="F195">
+        <v>838.89</v>
+      </c>
+      <c r="G195">
+        <v>762.87</v>
+      </c>
+      <c r="H195">
+        <v>704.66</v>
+      </c>
+      <c r="I195">
+        <v>673.12</v>
+      </c>
+      <c r="J195">
+        <v>665.74</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>11640</v>
+      </c>
+      <c r="B196">
+        <v>1086.9000000000001</v>
+      </c>
+      <c r="C196">
+        <v>1051.0999999999999</v>
+      </c>
+      <c r="D196">
+        <v>948.84</v>
+      </c>
+      <c r="E196">
+        <v>840.97</v>
+      </c>
+      <c r="F196">
+        <v>840.98</v>
+      </c>
+      <c r="G196">
+        <v>765.23</v>
+      </c>
+      <c r="H196">
+        <v>707.18</v>
+      </c>
+      <c r="I196">
+        <v>675.7</v>
+      </c>
+      <c r="J196">
+        <v>668.34</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>11700</v>
+      </c>
+      <c r="B197">
+        <v>1087.7</v>
+      </c>
+      <c r="C197">
+        <v>1052.2</v>
+      </c>
+      <c r="D197">
+        <v>950.46</v>
+      </c>
+      <c r="E197">
+        <v>843.06</v>
+      </c>
+      <c r="F197">
+        <v>843.07</v>
+      </c>
+      <c r="G197">
+        <v>767.57</v>
+      </c>
+      <c r="H197">
+        <v>709.69</v>
+      </c>
+      <c r="I197">
+        <v>678.28</v>
+      </c>
+      <c r="J197">
+        <v>670.93</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>11760</v>
+      </c>
+      <c r="B198">
+        <v>1088.5999999999999</v>
+      </c>
+      <c r="C198">
+        <v>1053.3</v>
+      </c>
+      <c r="D198">
+        <v>952.08</v>
+      </c>
+      <c r="E198">
+        <v>845.13</v>
+      </c>
+      <c r="F198">
+        <v>845.14</v>
+      </c>
+      <c r="G198">
+        <v>769.9</v>
+      </c>
+      <c r="H198">
+        <v>712.18</v>
+      </c>
+      <c r="I198">
+        <v>680.84</v>
+      </c>
+      <c r="J198">
+        <v>673.51</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>11820</v>
+      </c>
+      <c r="B199">
+        <v>1089.5</v>
+      </c>
+      <c r="C199">
+        <v>1054.3</v>
+      </c>
+      <c r="D199">
+        <v>953.68</v>
+      </c>
+      <c r="E199">
+        <v>847.19</v>
+      </c>
+      <c r="F199">
+        <v>847.2</v>
+      </c>
+      <c r="G199">
+        <v>772.22</v>
+      </c>
+      <c r="H199">
+        <v>714.66</v>
+      </c>
+      <c r="I199">
+        <v>683.39</v>
+      </c>
+      <c r="J199">
+        <v>676.07</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>11880</v>
+      </c>
+      <c r="B200">
+        <v>1090.3</v>
+      </c>
+      <c r="C200">
+        <v>1055.4000000000001</v>
+      </c>
+      <c r="D200">
+        <v>955.27</v>
+      </c>
+      <c r="E200">
+        <v>849.23</v>
+      </c>
+      <c r="F200">
+        <v>849.24</v>
+      </c>
+      <c r="G200">
+        <v>774.52</v>
+      </c>
+      <c r="H200">
+        <v>717.13</v>
+      </c>
+      <c r="I200">
+        <v>685.93</v>
+      </c>
+      <c r="J200">
+        <v>678.63</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>11940</v>
+      </c>
+      <c r="B201">
+        <v>1091.2</v>
+      </c>
+      <c r="C201">
+        <v>1056.5</v>
+      </c>
+      <c r="D201">
+        <v>956.85</v>
+      </c>
+      <c r="E201">
+        <v>851.27</v>
+      </c>
+      <c r="F201">
+        <v>851.28</v>
+      </c>
+      <c r="G201">
+        <v>776.82</v>
+      </c>
+      <c r="H201">
+        <v>719.59</v>
+      </c>
+      <c r="I201">
+        <v>688.45</v>
+      </c>
+      <c r="J201">
+        <v>681.17</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>12000</v>
+      </c>
+      <c r="B202">
+        <v>1092</v>
+      </c>
+      <c r="C202">
+        <v>1057.5</v>
+      </c>
+      <c r="D202">
+        <v>958.43</v>
+      </c>
+      <c r="E202">
+        <v>853.29</v>
+      </c>
+      <c r="F202">
+        <v>853.3</v>
+      </c>
+      <c r="G202">
+        <v>779.1</v>
+      </c>
+      <c r="H202">
+        <v>722.03</v>
+      </c>
+      <c r="I202">
+        <v>690.97</v>
+      </c>
+      <c r="J202">
+        <v>683.7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>12060</v>
+      </c>
+      <c r="B203">
+        <v>1092.9000000000001</v>
+      </c>
+      <c r="C203">
+        <v>1058.5</v>
+      </c>
+      <c r="D203">
+        <v>959.99</v>
+      </c>
+      <c r="E203">
+        <v>855.3</v>
+      </c>
+      <c r="F203">
+        <v>855.31</v>
+      </c>
+      <c r="G203">
+        <v>781.37</v>
+      </c>
+      <c r="H203">
+        <v>724.46</v>
+      </c>
+      <c r="I203">
+        <v>693.47</v>
+      </c>
+      <c r="J203">
+        <v>686.21</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>12120</v>
+      </c>
+      <c r="B204">
+        <v>1093.7</v>
+      </c>
+      <c r="C204">
+        <v>1059.5999999999999</v>
+      </c>
+      <c r="D204">
+        <v>961.54</v>
+      </c>
+      <c r="E204">
+        <v>857.3</v>
+      </c>
+      <c r="F204">
+        <v>857.31</v>
+      </c>
+      <c r="G204">
+        <v>783.63</v>
+      </c>
+      <c r="H204">
+        <v>726.88</v>
+      </c>
+      <c r="I204">
+        <v>695.96</v>
+      </c>
+      <c r="J204">
+        <v>688.72</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>12180</v>
+      </c>
+      <c r="B205">
+        <v>1094.5</v>
+      </c>
+      <c r="C205">
+        <v>1060.5999999999999</v>
+      </c>
+      <c r="D205">
+        <v>963.08</v>
+      </c>
+      <c r="E205">
+        <v>859.29</v>
+      </c>
+      <c r="F205">
+        <v>859.3</v>
+      </c>
+      <c r="G205">
+        <v>785.88</v>
+      </c>
+      <c r="H205">
+        <v>729.29</v>
+      </c>
+      <c r="I205">
+        <v>698.44</v>
+      </c>
+      <c r="J205">
+        <v>691.21</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>12240</v>
+      </c>
+      <c r="B206">
+        <v>1095.4000000000001</v>
+      </c>
+      <c r="C206">
+        <v>1061.5999999999999</v>
+      </c>
+      <c r="D206">
+        <v>964.61</v>
+      </c>
+      <c r="E206">
+        <v>861.27</v>
+      </c>
+      <c r="F206">
+        <v>861.28</v>
+      </c>
+      <c r="G206">
+        <v>788.11</v>
+      </c>
+      <c r="H206">
+        <v>731.68</v>
+      </c>
+      <c r="I206">
+        <v>700.91</v>
+      </c>
+      <c r="J206">
+        <v>693.69</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>12300</v>
+      </c>
+      <c r="B207">
+        <v>1096.2</v>
+      </c>
+      <c r="C207">
+        <v>1062.5999999999999</v>
+      </c>
+      <c r="D207">
+        <v>966.14</v>
+      </c>
+      <c r="E207">
+        <v>863.23</v>
+      </c>
+      <c r="F207">
+        <v>863.24</v>
+      </c>
+      <c r="G207">
+        <v>790.34</v>
+      </c>
+      <c r="H207">
+        <v>734.06</v>
+      </c>
+      <c r="I207">
+        <v>703.37</v>
+      </c>
+      <c r="J207">
+        <v>696.17</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>12360</v>
+      </c>
+      <c r="B208">
+        <v>1097</v>
+      </c>
+      <c r="C208">
+        <v>1063.5999999999999</v>
+      </c>
+      <c r="D208">
+        <v>967.65</v>
+      </c>
+      <c r="E208">
+        <v>865.19</v>
+      </c>
+      <c r="F208">
+        <v>865.2</v>
+      </c>
+      <c r="G208">
+        <v>792.55</v>
+      </c>
+      <c r="H208">
+        <v>736.43</v>
+      </c>
+      <c r="I208">
+        <v>705.81</v>
+      </c>
+      <c r="J208">
+        <v>698.63</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>12420</v>
+      </c>
+      <c r="B209">
+        <v>1097.8</v>
+      </c>
+      <c r="C209">
+        <v>1064.5999999999999</v>
+      </c>
+      <c r="D209">
+        <v>969.15</v>
+      </c>
+      <c r="E209">
+        <v>867.13</v>
+      </c>
+      <c r="F209">
+        <v>867.14</v>
+      </c>
+      <c r="G209">
+        <v>794.75</v>
+      </c>
+      <c r="H209">
+        <v>738.79</v>
+      </c>
+      <c r="I209">
+        <v>708.25</v>
+      </c>
+      <c r="J209">
+        <v>701.07</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>12480</v>
+      </c>
+      <c r="B210">
+        <v>1098.5999999999999</v>
+      </c>
+      <c r="C210">
+        <v>1065.5999999999999</v>
+      </c>
+      <c r="D210">
+        <v>970.65</v>
+      </c>
+      <c r="E210">
+        <v>869.06</v>
+      </c>
+      <c r="F210">
+        <v>869.07</v>
+      </c>
+      <c r="G210">
+        <v>796.95</v>
+      </c>
+      <c r="H210">
+        <v>741.14</v>
+      </c>
+      <c r="I210">
+        <v>710.67</v>
+      </c>
+      <c r="J210">
+        <v>703.51</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>12540</v>
+      </c>
+      <c r="B211">
+        <v>1099.4000000000001</v>
+      </c>
+      <c r="C211">
+        <v>1066.5999999999999</v>
+      </c>
+      <c r="D211">
+        <v>972.13</v>
+      </c>
+      <c r="E211">
+        <v>870.99</v>
+      </c>
+      <c r="F211">
+        <v>870.99</v>
+      </c>
+      <c r="G211">
+        <v>799.13</v>
+      </c>
+      <c r="H211">
+        <v>743.47</v>
+      </c>
+      <c r="I211">
+        <v>713.09</v>
+      </c>
+      <c r="J211">
+        <v>705.94</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>12600</v>
+      </c>
+      <c r="B212">
+        <v>1100.2</v>
+      </c>
+      <c r="C212">
+        <v>1067.5999999999999</v>
+      </c>
+      <c r="D212">
+        <v>973.6</v>
+      </c>
+      <c r="E212">
+        <v>872.9</v>
+      </c>
+      <c r="F212">
+        <v>872.91</v>
+      </c>
+      <c r="G212">
+        <v>801.3</v>
+      </c>
+      <c r="H212">
+        <v>745.79</v>
+      </c>
+      <c r="I212">
+        <v>715.49</v>
+      </c>
+      <c r="J212">
+        <v>708.36</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>12660</v>
+      </c>
+      <c r="B213">
+        <v>1100.9000000000001</v>
+      </c>
+      <c r="C213">
+        <v>1068.5</v>
+      </c>
+      <c r="D213">
+        <v>975.07</v>
+      </c>
+      <c r="E213">
+        <v>874.8</v>
+      </c>
+      <c r="F213">
+        <v>874.81</v>
+      </c>
+      <c r="G213">
+        <v>803.46</v>
+      </c>
+      <c r="H213">
+        <v>748.11</v>
+      </c>
+      <c r="I213">
+        <v>717.88</v>
+      </c>
+      <c r="J213">
+        <v>710.77</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>12720</v>
+      </c>
+      <c r="B214">
+        <v>1101.7</v>
+      </c>
+      <c r="C214">
+        <v>1069.5</v>
+      </c>
+      <c r="D214">
+        <v>976.52</v>
+      </c>
+      <c r="E214">
+        <v>876.69</v>
+      </c>
+      <c r="F214">
+        <v>876.69</v>
+      </c>
+      <c r="G214">
+        <v>805.61</v>
+      </c>
+      <c r="H214">
+        <v>750.41</v>
+      </c>
+      <c r="I214">
+        <v>720.26</v>
+      </c>
+      <c r="J214">
+        <v>713.16</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>12780</v>
+      </c>
+      <c r="B215">
+        <v>1102.5</v>
+      </c>
+      <c r="C215">
+        <v>1070.5</v>
+      </c>
+      <c r="D215">
+        <v>977.97</v>
+      </c>
+      <c r="E215">
+        <v>878.57</v>
+      </c>
+      <c r="F215">
+        <v>878.57</v>
+      </c>
+      <c r="G215">
+        <v>807.74</v>
+      </c>
+      <c r="H215">
+        <v>752.7</v>
+      </c>
+      <c r="I215">
+        <v>722.63</v>
+      </c>
+      <c r="J215">
+        <v>715.55</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>12840</v>
+      </c>
+      <c r="B216">
+        <v>1103.3</v>
+      </c>
+      <c r="C216">
+        <v>1071.4000000000001</v>
+      </c>
+      <c r="D216">
+        <v>979.41</v>
+      </c>
+      <c r="E216">
+        <v>880.43</v>
+      </c>
+      <c r="F216">
+        <v>880.44</v>
+      </c>
+      <c r="G216">
+        <v>809.87</v>
+      </c>
+      <c r="H216">
+        <v>754.97</v>
+      </c>
+      <c r="I216">
+        <v>724.98</v>
+      </c>
+      <c r="J216">
+        <v>717.92</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>12900</v>
+      </c>
+      <c r="B217">
+        <v>1104</v>
+      </c>
+      <c r="C217">
+        <v>1072.4000000000001</v>
+      </c>
+      <c r="D217">
+        <v>980.84</v>
+      </c>
+      <c r="E217">
+        <v>882.29</v>
+      </c>
+      <c r="F217">
+        <v>882.3</v>
+      </c>
+      <c r="G217">
+        <v>811.98</v>
+      </c>
+      <c r="H217">
+        <v>757.24</v>
+      </c>
+      <c r="I217">
+        <v>727.33</v>
+      </c>
+      <c r="J217">
+        <v>720.29</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>12960</v>
+      </c>
+      <c r="B218">
+        <v>1104.8</v>
+      </c>
+      <c r="C218">
+        <v>1073.3</v>
+      </c>
+      <c r="D218">
+        <v>982.26</v>
+      </c>
+      <c r="E218">
+        <v>884.14</v>
+      </c>
+      <c r="F218">
+        <v>884.15</v>
+      </c>
+      <c r="G218">
+        <v>814.08</v>
+      </c>
+      <c r="H218">
+        <v>759.5</v>
+      </c>
+      <c r="I218">
+        <v>729.67</v>
+      </c>
+      <c r="J218">
+        <v>722.64</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>13020</v>
+      </c>
+      <c r="B219">
+        <v>1105.5999999999999</v>
+      </c>
+      <c r="C219">
+        <v>1074.2</v>
+      </c>
+      <c r="D219">
+        <v>983.67</v>
+      </c>
+      <c r="E219">
+        <v>885.98</v>
+      </c>
+      <c r="F219">
+        <v>885.99</v>
+      </c>
+      <c r="G219">
+        <v>816.17</v>
+      </c>
+      <c r="H219">
+        <v>761.75</v>
+      </c>
+      <c r="I219">
+        <v>731.99</v>
+      </c>
+      <c r="J219">
+        <v>724.98</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>13080</v>
+      </c>
+      <c r="B220">
+        <v>1106.3</v>
+      </c>
+      <c r="C220">
+        <v>1075.2</v>
+      </c>
+      <c r="D220">
+        <v>985.07</v>
+      </c>
+      <c r="E220">
+        <v>887.81</v>
+      </c>
+      <c r="F220">
+        <v>887.81</v>
+      </c>
+      <c r="G220">
+        <v>818.25</v>
+      </c>
+      <c r="H220">
+        <v>763.98</v>
+      </c>
+      <c r="I220">
+        <v>734.3</v>
+      </c>
+      <c r="J220">
+        <v>727.32</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>13140</v>
+      </c>
+      <c r="B221">
+        <v>1107.0999999999999</v>
+      </c>
+      <c r="C221">
+        <v>1076.0999999999999</v>
+      </c>
+      <c r="D221">
+        <v>986.46</v>
+      </c>
+      <c r="E221">
+        <v>889.62</v>
+      </c>
+      <c r="F221">
+        <v>889.63</v>
+      </c>
+      <c r="G221">
+        <v>820.32</v>
+      </c>
+      <c r="H221">
+        <v>766.21</v>
+      </c>
+      <c r="I221">
+        <v>736.61</v>
+      </c>
+      <c r="J221">
+        <v>729.64</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>13200</v>
+      </c>
+      <c r="B222">
+        <v>1107.8</v>
+      </c>
+      <c r="C222">
+        <v>1077</v>
+      </c>
+      <c r="D222">
+        <v>987.85</v>
+      </c>
+      <c r="E222">
+        <v>891.43</v>
+      </c>
+      <c r="F222">
+        <v>891.44</v>
+      </c>
+      <c r="G222">
+        <v>822.38</v>
+      </c>
+      <c r="H222">
+        <v>768.42</v>
+      </c>
+      <c r="I222">
+        <v>738.9</v>
+      </c>
+      <c r="J222">
+        <v>731.95</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>13260</v>
+      </c>
+      <c r="B223">
+        <v>1108.5999999999999</v>
+      </c>
+      <c r="C223">
+        <v>1077.9000000000001</v>
+      </c>
+      <c r="D223">
+        <v>989.23</v>
+      </c>
+      <c r="E223">
+        <v>893.23</v>
+      </c>
+      <c r="F223">
+        <v>893.24</v>
+      </c>
+      <c r="G223">
+        <v>824.43</v>
+      </c>
+      <c r="H223">
+        <v>770.62</v>
+      </c>
+      <c r="I223">
+        <v>741.18</v>
+      </c>
+      <c r="J223">
+        <v>734.25</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>13320</v>
+      </c>
+      <c r="B224">
+        <v>1109.3</v>
+      </c>
+      <c r="C224">
+        <v>1078.8</v>
+      </c>
+      <c r="D224">
+        <v>990.6</v>
+      </c>
+      <c r="E224">
+        <v>895.02</v>
+      </c>
+      <c r="F224">
+        <v>895.03</v>
+      </c>
+      <c r="G224">
+        <v>826.47</v>
+      </c>
+      <c r="H224">
+        <v>772.82</v>
+      </c>
+      <c r="I224">
+        <v>743.45</v>
+      </c>
+      <c r="J224">
+        <v>736.54</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>13380</v>
+      </c>
+      <c r="B225">
+        <v>1110</v>
+      </c>
+      <c r="C225">
+        <v>1079.7</v>
+      </c>
+      <c r="D225">
+        <v>991.96</v>
+      </c>
+      <c r="E225">
+        <v>896.8</v>
+      </c>
+      <c r="F225">
+        <v>896.81</v>
+      </c>
+      <c r="G225">
+        <v>828.49</v>
+      </c>
+      <c r="H225">
+        <v>775</v>
+      </c>
+      <c r="I225">
+        <v>745.71</v>
+      </c>
+      <c r="J225">
+        <v>738.81</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>13440</v>
+      </c>
+      <c r="B226">
+        <v>1110.8</v>
+      </c>
+      <c r="C226">
+        <v>1080.5999999999999</v>
+      </c>
+      <c r="D226">
+        <v>993.31</v>
+      </c>
+      <c r="E226">
+        <v>898.57</v>
+      </c>
+      <c r="F226">
+        <v>898.58</v>
+      </c>
+      <c r="G226">
+        <v>830.51</v>
+      </c>
+      <c r="H226">
+        <v>777.18</v>
+      </c>
+      <c r="I226">
+        <v>747.96</v>
+      </c>
+      <c r="J226">
+        <v>741.08</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>13500</v>
+      </c>
+      <c r="B227">
+        <v>1111.5</v>
+      </c>
+      <c r="C227">
+        <v>1081.5</v>
+      </c>
+      <c r="D227">
+        <v>994.66</v>
+      </c>
+      <c r="E227">
+        <v>900.33</v>
+      </c>
+      <c r="F227">
+        <v>900.34</v>
+      </c>
+      <c r="G227">
+        <v>832.51</v>
+      </c>
+      <c r="H227">
+        <v>779.34</v>
+      </c>
+      <c r="I227">
+        <v>750.2</v>
+      </c>
+      <c r="J227">
+        <v>743.34</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>13560</v>
+      </c>
+      <c r="B228">
+        <v>1112.2</v>
+      </c>
+      <c r="C228">
+        <v>1082.4000000000001</v>
+      </c>
+      <c r="D228">
+        <v>995.99</v>
+      </c>
+      <c r="E228">
+        <v>902.08</v>
+      </c>
+      <c r="F228">
+        <v>902.09</v>
+      </c>
+      <c r="G228">
+        <v>834.51</v>
+      </c>
+      <c r="H228">
+        <v>781.49</v>
+      </c>
+      <c r="I228">
+        <v>752.43</v>
+      </c>
+      <c r="J228">
+        <v>745.59</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>13620</v>
+      </c>
+      <c r="B229">
+        <v>1112.9000000000001</v>
+      </c>
+      <c r="C229">
+        <v>1083.3</v>
+      </c>
+      <c r="D229">
+        <v>997.32</v>
+      </c>
+      <c r="E229">
+        <v>903.82</v>
+      </c>
+      <c r="F229">
+        <v>903.83</v>
+      </c>
+      <c r="G229">
+        <v>836.49</v>
+      </c>
+      <c r="H229">
+        <v>783.64</v>
+      </c>
+      <c r="I229">
+        <v>754.65</v>
+      </c>
+      <c r="J229">
+        <v>747.82</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>13680</v>
+      </c>
+      <c r="B230">
+        <v>1113.7</v>
+      </c>
+      <c r="C230">
+        <v>1084.2</v>
+      </c>
+      <c r="D230">
+        <v>998.64</v>
+      </c>
+      <c r="E230">
+        <v>905.55</v>
+      </c>
+      <c r="F230">
+        <v>905.56</v>
+      </c>
+      <c r="G230">
+        <v>838.46</v>
+      </c>
+      <c r="H230">
+        <v>785.77</v>
+      </c>
+      <c r="I230">
+        <v>756.86</v>
+      </c>
+      <c r="J230">
+        <v>750.05</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>13740</v>
+      </c>
+      <c r="B231">
+        <v>1114.4000000000001</v>
+      </c>
+      <c r="C231">
+        <v>1085</v>
+      </c>
+      <c r="D231">
+        <v>999.96</v>
+      </c>
+      <c r="E231">
+        <v>907.27</v>
+      </c>
+      <c r="F231">
+        <v>907.28</v>
+      </c>
+      <c r="G231">
+        <v>840.43</v>
+      </c>
+      <c r="H231">
+        <v>787.9</v>
+      </c>
+      <c r="I231">
+        <v>759.06</v>
+      </c>
+      <c r="J231">
+        <v>752.26</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>13800</v>
+      </c>
+      <c r="B232">
+        <v>1115.0999999999999</v>
+      </c>
+      <c r="C232">
+        <v>1085.9000000000001</v>
+      </c>
+      <c r="D232">
+        <v>1001.3</v>
+      </c>
+      <c r="E232">
+        <v>908.98</v>
+      </c>
+      <c r="F232">
+        <v>908.99</v>
+      </c>
+      <c r="G232">
+        <v>842.38</v>
+      </c>
+      <c r="H232">
+        <v>790.01</v>
+      </c>
+      <c r="I232">
+        <v>761.24</v>
+      </c>
+      <c r="J232">
+        <v>754.47</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>13860</v>
+      </c>
+      <c r="B233">
+        <v>1115.8</v>
+      </c>
+      <c r="C233">
+        <v>1086.8</v>
+      </c>
+      <c r="D233">
+        <v>1002.6</v>
+      </c>
+      <c r="E233">
+        <v>910.69</v>
+      </c>
+      <c r="F233">
+        <v>910.69</v>
+      </c>
+      <c r="G233">
+        <v>844.32</v>
+      </c>
+      <c r="H233">
+        <v>792.12</v>
+      </c>
+      <c r="I233">
+        <v>763.42</v>
+      </c>
+      <c r="J233">
+        <v>756.67</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>13920</v>
+      </c>
+      <c r="B234">
+        <v>1116.5</v>
+      </c>
+      <c r="C234">
+        <v>1087.5999999999999</v>
+      </c>
+      <c r="D234">
+        <v>1003.9</v>
+      </c>
+      <c r="E234">
+        <v>912.38</v>
+      </c>
+      <c r="F234">
+        <v>912.39</v>
+      </c>
+      <c r="G234">
+        <v>846.26</v>
+      </c>
+      <c r="H234">
+        <v>794.21</v>
+      </c>
+      <c r="I234">
+        <v>765.59</v>
+      </c>
+      <c r="J234">
+        <v>758.85</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>13980</v>
+      </c>
+      <c r="B235">
+        <v>1117.2</v>
+      </c>
+      <c r="C235">
+        <v>1088.5</v>
+      </c>
+      <c r="D235">
+        <v>1005.1</v>
+      </c>
+      <c r="E235">
+        <v>914.06</v>
+      </c>
+      <c r="F235">
+        <v>914.07</v>
+      </c>
+      <c r="G235">
+        <v>848.18</v>
+      </c>
+      <c r="H235">
+        <v>796.3</v>
+      </c>
+      <c r="I235">
+        <v>767.75</v>
+      </c>
+      <c r="J235">
+        <v>761.03</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>14040</v>
+      </c>
+      <c r="B236">
+        <v>1117.9000000000001</v>
+      </c>
+      <c r="C236">
+        <v>1089.4000000000001</v>
+      </c>
+      <c r="D236">
+        <v>1006.4</v>
+      </c>
+      <c r="E236">
+        <v>915.74</v>
+      </c>
+      <c r="F236">
+        <v>915.74</v>
+      </c>
+      <c r="G236">
+        <v>850.1</v>
+      </c>
+      <c r="H236">
+        <v>798.38</v>
+      </c>
+      <c r="I236">
+        <v>769.9</v>
+      </c>
+      <c r="J236">
+        <v>763.19</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>14100</v>
+      </c>
+      <c r="B237">
+        <v>1118.5999999999999</v>
+      </c>
+      <c r="C237">
+        <v>1090.2</v>
+      </c>
+      <c r="D237">
+        <v>1007.7</v>
+      </c>
+      <c r="E237">
+        <v>917.4</v>
+      </c>
+      <c r="F237">
+        <v>917.41</v>
+      </c>
+      <c r="G237">
+        <v>852</v>
+      </c>
+      <c r="H237">
+        <v>800.45</v>
+      </c>
+      <c r="I237">
+        <v>772.04</v>
+      </c>
+      <c r="J237">
+        <v>765.35</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>14160</v>
+      </c>
+      <c r="B238">
+        <v>1119.3</v>
+      </c>
+      <c r="C238">
+        <v>1091</v>
+      </c>
+      <c r="D238">
+        <v>1008.9</v>
+      </c>
+      <c r="E238">
+        <v>919.06</v>
+      </c>
+      <c r="F238">
+        <v>919.07</v>
+      </c>
+      <c r="G238">
+        <v>853.9</v>
+      </c>
+      <c r="H238">
+        <v>802.51</v>
+      </c>
+      <c r="I238">
+        <v>774.17</v>
+      </c>
+      <c r="J238">
+        <v>767.5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>14220</v>
+      </c>
+      <c r="B239">
+        <v>1120</v>
+      </c>
+      <c r="C239">
+        <v>1091.9000000000001</v>
+      </c>
+      <c r="D239">
+        <v>1010.2</v>
+      </c>
+      <c r="E239">
+        <v>920.7</v>
+      </c>
+      <c r="F239">
+        <v>920.71</v>
+      </c>
+      <c r="G239">
+        <v>855.78</v>
+      </c>
+      <c r="H239">
+        <v>804.56</v>
+      </c>
+      <c r="I239">
+        <v>776.29</v>
+      </c>
+      <c r="J239">
+        <v>769.64</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>14280</v>
+      </c>
+      <c r="B240">
+        <v>1120.7</v>
+      </c>
+      <c r="C240">
+        <v>1092.7</v>
+      </c>
+      <c r="D240">
+        <v>1011.4</v>
+      </c>
+      <c r="E240">
+        <v>922.34</v>
+      </c>
+      <c r="F240">
+        <v>922.35</v>
+      </c>
+      <c r="G240">
+        <v>857.66</v>
+      </c>
+      <c r="H240">
+        <v>806.6</v>
+      </c>
+      <c r="I240">
+        <v>778.4</v>
+      </c>
+      <c r="J240">
+        <v>771.76</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>14340</v>
+      </c>
+      <c r="B241">
+        <v>1121.4000000000001</v>
+      </c>
+      <c r="C241">
+        <v>1093.5999999999999</v>
+      </c>
+      <c r="D241">
+        <v>1012.7</v>
+      </c>
+      <c r="E241">
+        <v>923.97</v>
+      </c>
+      <c r="F241">
+        <v>923.98</v>
+      </c>
+      <c r="G241">
+        <v>859.53</v>
+      </c>
+      <c r="H241">
+        <v>808.63</v>
+      </c>
+      <c r="I241">
+        <v>780.5</v>
+      </c>
+      <c r="J241">
+        <v>773.88</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>14400</v>
+      </c>
+      <c r="B242">
+        <v>1122</v>
+      </c>
+      <c r="C242">
+        <v>1094.4000000000001</v>
+      </c>
+      <c r="D242">
+        <v>1013.9</v>
+      </c>
+      <c r="E242">
+        <v>925.59</v>
+      </c>
+      <c r="F242">
+        <v>925.6</v>
+      </c>
+      <c r="G242">
+        <v>861.38</v>
+      </c>
+      <c r="H242">
+        <v>810.65</v>
+      </c>
+      <c r="I242">
+        <v>782.6</v>
+      </c>
+      <c r="J242">
+        <v>775.99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>